<commit_message>
PZR 8 cviceni dodelat
</commit_message>
<xml_diff>
--- a/2/PZS/6/kruhovaKonv.xlsx
+++ b/2/PZS/6/kruhovaKonv.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26227"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{936BB81B-31D6-4087-9A10-2B89043E9BF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -87,18 +88,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normální" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -114,7 +113,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motiv Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -189,6 +188,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -224,6 +240,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -399,11 +432,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:Z24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -572,48 +605,48 @@
       </c>
     </row>
     <row r="11" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="G11" s="4">
-        <v>0</v>
-      </c>
-      <c r="H11" s="4">
-        <v>1</v>
-      </c>
-      <c r="I11" s="4">
-        <v>4</v>
-      </c>
-      <c r="J11" s="4">
-        <v>5</v>
-      </c>
-      <c r="K11" s="4">
-        <v>5</v>
-      </c>
-      <c r="L11" s="4">
+      <c r="G11" s="1">
+        <v>0</v>
+      </c>
+      <c r="H11" s="1">
+        <v>1</v>
+      </c>
+      <c r="I11" s="1">
+        <v>4</v>
+      </c>
+      <c r="J11" s="1">
+        <v>5</v>
+      </c>
+      <c r="K11" s="1">
+        <v>5</v>
+      </c>
+      <c r="L11" s="1">
         <v>6</v>
       </c>
-      <c r="M11" s="4">
+      <c r="M11" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="K12" s="5">
-        <v>0</v>
-      </c>
-      <c r="L12" s="5">
-        <v>1</v>
-      </c>
-      <c r="M12" s="5">
-        <v>4</v>
-      </c>
-      <c r="N12" s="5">
-        <v>5</v>
-      </c>
-      <c r="O12" s="5">
-        <v>5</v>
-      </c>
-      <c r="P12" s="5">
+      <c r="K12" s="2">
+        <v>0</v>
+      </c>
+      <c r="L12" s="2">
+        <v>1</v>
+      </c>
+      <c r="M12" s="2">
+        <v>4</v>
+      </c>
+      <c r="N12" s="2">
+        <v>5</v>
+      </c>
+      <c r="O12" s="2">
+        <v>5</v>
+      </c>
+      <c r="P12" s="2">
         <v>6</v>
       </c>
-      <c r="Q12" s="5">
+      <c r="Q12" s="2">
         <v>3</v>
       </c>
     </row>
@@ -622,7 +655,7 @@
         <v>0</v>
       </c>
       <c r="D13" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13" s="3">
         <v>4</v>
@@ -630,28 +663,28 @@
       <c r="F13" s="3">
         <v>5</v>
       </c>
-      <c r="G13" s="6">
-        <v>5</v>
-      </c>
-      <c r="H13" s="6">
+      <c r="G13" s="4">
+        <v>5</v>
+      </c>
+      <c r="H13" s="4">
         <v>7</v>
       </c>
-      <c r="I13" s="6">
+      <c r="I13" s="4">
         <v>7</v>
       </c>
-      <c r="J13" s="6">
-        <v>5</v>
-      </c>
-      <c r="K13" s="7">
-        <v>5</v>
-      </c>
-      <c r="L13" s="7">
+      <c r="J13" s="4">
+        <v>5</v>
+      </c>
+      <c r="K13" s="5">
+        <v>5</v>
+      </c>
+      <c r="L13" s="5">
         <v>7</v>
       </c>
-      <c r="M13" s="7">
+      <c r="M13" s="5">
         <v>7</v>
       </c>
-      <c r="N13" s="7">
+      <c r="N13" s="5">
         <v>5</v>
       </c>
       <c r="O13" s="3">

</xml_diff>